<commit_message>
Se arreglo el sprint backlog y el burndown chart
</commit_message>
<xml_diff>
--- a/Fase2/Evidencias Proyecto/Sprint 0 - Sprint Backlog & Burndown Chart.xlsx
+++ b/Fase2/Evidencias Proyecto/Sprint 0 - Sprint Backlog & Burndown Chart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t>SPRINT BACKLOG &amp; BURNDOWN CHART</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Completar Acta de Sprint Retrospective</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Generación de Trello</t>
   </si>
   <si>
@@ -175,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="39">
     <border/>
     <border>
       <left style="medium">
@@ -457,14 +454,6 @@
       </top>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
       <left style="thick">
         <color rgb="FF000000"/>
       </left>
@@ -606,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -617,10 +606,20 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="7" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -655,25 +654,22 @@
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="18" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="19" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="20" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="21" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="22" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="23" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
@@ -681,7 +677,7 @@
     <xf borderId="24" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="22" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="24" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="24" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -693,27 +689,21 @@
     <xf borderId="26" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="27" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="25" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
     <xf borderId="25" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="28" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="27" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="29" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="28" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="29" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="30" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="31" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="32" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="31" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="33" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="32" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="19" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -728,20 +718,20 @@
     <xf borderId="4" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="34" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="33" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="34" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="35" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="36" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="37" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="37" fillId="4" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="38" fillId="4" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="39" fillId="4" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -847,11 +837,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1742508071"/>
-        <c:axId val="2043468220"/>
+        <c:axId val="580799995"/>
+        <c:axId val="322676877"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1742508071"/>
+        <c:axId val="580799995"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -903,10 +893,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2043468220"/>
+        <c:crossAx val="322676877"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2043468220"/>
+        <c:axId val="322676877"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -970,7 +960,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1742508071"/>
+        <c:crossAx val="580799995"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1000,10 +990,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>771525</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="7543800" cy="3971925"/>
     <xdr:graphicFrame>
@@ -1226,7 +1216,10 @@
     <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="7.0" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection activeCell="I2" sqref="I2" pane="topRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
@@ -1280,13 +1273,13 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="5"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -1305,19 +1298,19 @@
     </row>
     <row r="3">
       <c r="A3" s="1"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -1367,43 +1360,43 @@
     </row>
     <row r="5">
       <c r="A5" s="1"/>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="L5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="M5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="14" t="s">
+      <c r="N5" s="16" t="s">
         <v>13</v>
       </c>
       <c r="O5" s="1"/>
@@ -1424,37 +1417,43 @@
     </row>
     <row r="6" ht="25.5" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="22">
         <v>8.0</v>
       </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21">
+      <c r="H6" s="23">
+        <v>1.0</v>
+      </c>
+      <c r="I6" s="23">
+        <v>1.0</v>
+      </c>
+      <c r="J6" s="23">
+        <v>1.0</v>
+      </c>
+      <c r="K6" s="23">
+        <v>1.0</v>
+      </c>
+      <c r="L6" s="23">
         <v>1.5</v>
       </c>
-      <c r="M6" s="21">
+      <c r="M6" s="23">
         <v>1.0</v>
       </c>
-      <c r="N6" s="22">
-        <v>2.0</v>
-      </c>
+      <c r="N6" s="24"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
@@ -1473,33 +1472,33 @@
     </row>
     <row r="7">
       <c r="A7" s="1"/>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="24">
-        <v>3.0</v>
-      </c>
-      <c r="H7" s="25">
+      <c r="G7" s="26">
         <v>2.0</v>
       </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="27"/>
+      <c r="H7" s="19">
+        <v>2.0</v>
+      </c>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="28"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -1518,37 +1517,33 @@
     </row>
     <row r="8">
       <c r="A8" s="1"/>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="24">
-        <v>10.0</v>
-      </c>
-      <c r="H8" s="25">
+      <c r="G8" s="26">
         <v>2.0</v>
       </c>
-      <c r="I8" s="25">
-        <v>3.0</v>
-      </c>
-      <c r="J8" s="25">
+      <c r="H8" s="19">
         <v>2.0</v>
       </c>
-      <c r="K8" s="25"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="27"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="28"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -1567,33 +1562,39 @@
     </row>
     <row r="9">
       <c r="A9" s="1"/>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="26">
         <v>8.0</v>
       </c>
-      <c r="H9" s="25"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="25">
+      <c r="H9" s="19"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="19">
         <v>4.0</v>
       </c>
-      <c r="K9" s="25"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="27"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="M9" s="19">
+        <v>2.0</v>
+      </c>
+      <c r="N9" s="29">
+        <v>1.0</v>
+      </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
@@ -1612,35 +1613,35 @@
     </row>
     <row r="10">
       <c r="A10" s="1"/>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="26">
         <v>6.0</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="19">
         <v>3.0</v>
       </c>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25">
+      <c r="I10" s="19"/>
+      <c r="J10" s="19">
         <v>3.0</v>
       </c>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="28"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
@@ -1659,34 +1660,40 @@
     </row>
     <row r="11">
       <c r="A11" s="1"/>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="26">
         <v>5.0</v>
       </c>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="25">
+      <c r="H11" s="19">
         <v>1.0</v>
       </c>
-      <c r="K11" s="25">
+      <c r="I11" s="19">
         <v>1.0</v>
       </c>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
+      <c r="J11" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="K11" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="L11" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="M11" s="19"/>
       <c r="N11" s="29"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -1706,35 +1713,37 @@
     </row>
     <row r="12">
       <c r="A12" s="1"/>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="26">
         <v>2.0</v>
       </c>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25">
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19">
         <v>1.5</v>
       </c>
-      <c r="M12" s="25">
+      <c r="M12" s="19">
         <v>1.0</v>
       </c>
-      <c r="N12" s="27"/>
+      <c r="N12" s="30">
+        <v>1.0</v>
+      </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -1753,34 +1762,32 @@
     </row>
     <row r="13">
       <c r="A13" s="1"/>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="26">
         <v>2.0</v>
       </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="25" t="s">
-        <v>28</v>
-      </c>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
       <c r="N13" s="29">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -1800,33 +1807,33 @@
     </row>
     <row r="14">
       <c r="A14" s="1"/>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="30" t="s">
-        <v>29</v>
+      <c r="D14" s="31" t="s">
+        <v>28</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F14" s="25" t="s">
         <v>20</v>
       </c>
       <c r="G14" s="32">
         <v>2.0</v>
       </c>
-      <c r="H14" s="33">
-        <v>1.5</v>
+      <c r="H14" s="31">
+        <v>2.0</v>
       </c>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="35"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="34"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
@@ -1845,44 +1852,44 @@
     </row>
     <row r="15">
       <c r="A15" s="1"/>
-      <c r="B15" s="36" t="s">
-        <v>30</v>
+      <c r="B15" s="35" t="s">
+        <v>29</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="41">
+      <c r="C15" s="36"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="40">
         <f>SUM(G6:G14)</f>
-        <v>46</v>
+        <v>37</v>
       </c>
-      <c r="H15" s="42">
+      <c r="H15" s="41">
         <f t="shared" ref="H15:N15" si="1">G15-SUM(H6:H14)</f>
-        <v>37.5</v>
+        <v>26</v>
       </c>
-      <c r="I15" s="42">
+      <c r="I15" s="41">
         <f t="shared" si="1"/>
-        <v>34.5</v>
+        <v>24</v>
       </c>
-      <c r="J15" s="42">
+      <c r="J15" s="41">
         <f t="shared" si="1"/>
-        <v>24.5</v>
+        <v>15</v>
       </c>
-      <c r="K15" s="42">
+      <c r="K15" s="41">
         <f t="shared" si="1"/>
-        <v>23.5</v>
+        <v>13</v>
       </c>
-      <c r="L15" s="42">
+      <c r="L15" s="41">
         <f t="shared" si="1"/>
-        <v>20.5</v>
+        <v>8</v>
       </c>
-      <c r="M15" s="42">
+      <c r="M15" s="41">
         <f t="shared" si="1"/>
-        <v>18.5</v>
+        <v>4</v>
       </c>
-      <c r="N15" s="43">
+      <c r="N15" s="42">
         <f t="shared" si="1"/>
-        <v>15.5</v>
+        <v>0</v>
       </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1902,42 +1909,42 @@
     </row>
     <row r="16">
       <c r="A16" s="1"/>
-      <c r="B16" s="44" t="s">
-        <v>31</v>
+      <c r="B16" s="43" t="s">
+        <v>30</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="48">
+      <c r="C16" s="7"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="47">
         <f>SUM(G6:G14)</f>
-        <v>46</v>
+        <v>37</v>
       </c>
-      <c r="H16" s="49">
+      <c r="H16" s="48">
         <f>$G$16-($G$16/7*1)</f>
-        <v>39.42857143</v>
+        <v>31.71428571</v>
       </c>
-      <c r="I16" s="49">
+      <c r="I16" s="48">
         <f>$G$16-($G$16/7*2)</f>
-        <v>32.85714286</v>
+        <v>26.42857143</v>
       </c>
-      <c r="J16" s="49">
+      <c r="J16" s="48">
         <f>$G$16-($G$16/7*3)</f>
-        <v>26.28571429</v>
+        <v>21.14285714</v>
       </c>
-      <c r="K16" s="49">
+      <c r="K16" s="48">
         <f>$G$16-($G$16/7*4)</f>
-        <v>19.71428571</v>
+        <v>15.85714286</v>
       </c>
-      <c r="L16" s="49">
+      <c r="L16" s="48">
         <f>$G$16-($G$16/7*5)</f>
-        <v>13.14285714</v>
+        <v>10.57142857</v>
       </c>
-      <c r="M16" s="49">
+      <c r="M16" s="48">
         <f>$G$16-($G$16/7*6)</f>
-        <v>6.571428571</v>
+        <v>5.285714286</v>
       </c>
-      <c r="N16" s="50">
+      <c r="N16" s="49">
         <f>$G$16-($G$16/7*7)</f>
         <v>0</v>
       </c>
@@ -2220,7 +2227,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
-      <c r="O25" s="51"/>
+      <c r="O25" s="50"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
@@ -32463,9 +32470,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B2:N3"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B2:G3"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>